<commit_message>
Add TOC to README and make minor modifications to dataset
</commit_message>
<xml_diff>
--- a/data/Colorado-Transbasin-Diversions.xlsx
+++ b/data/Colorado-Transbasin-Diversions.xlsx
@@ -3115,7 +3115,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y1" sqref="Y1"/>
+      <selection pane="bottomRight" activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7742,7 +7742,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>